<commit_message>
Several gas meter updated for UEF
</commit_message>
<xml_diff>
--- a/NI-2010/Drivers/Ritter Gas Meter/Documentation/Ritter Calibration Points.xlsx
+++ b/NI-2010/Drivers/Ritter Gas Meter/Documentation/Ritter Calibration Points.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Drivers\Ritter Gas Meter\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6E0C68-3000-4126-A461-09E3305CDF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09872ADE-F1F8-4C70-AC43-7C50F3B02F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1C82D58-A921-44CD-A08A-58376626D3EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D1C82D58-A921-44CD-A08A-58376626D3EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calibration Procedure" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="1.544.7HI" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="53">
   <si>
     <t>Flow Rate (Liters/Hour)</t>
   </si>
@@ -66,6 +69,135 @@
   </si>
   <si>
     <t>Totalized Flow (Liters)</t>
+  </si>
+  <si>
+    <t>Totalized Flow (L)-Ideal</t>
+  </si>
+  <si>
+    <t>Total Flow - cuft (0.5 Hours)</t>
+  </si>
+  <si>
+    <t>Total Flow - L (0.5 Hours)</t>
+  </si>
+  <si>
+    <t>Runtime (Minutes)</t>
+  </si>
+  <si>
+    <t>Propane Pilot</t>
+  </si>
+  <si>
+    <t>Natural Pilot</t>
+  </si>
+  <si>
+    <t>Propane Main Burner</t>
+  </si>
+  <si>
+    <t>Natural Main Burner</t>
+  </si>
+  <si>
+    <t>Natural PV Main Burner</t>
+  </si>
+  <si>
+    <t>TG10/4 Ritter Gas Flow Rate Calibration</t>
+  </si>
+  <si>
+    <t>TG3/1 Ritter Gas Flow Rate Calibration</t>
+  </si>
+  <si>
+    <t>TG3/1 Ritter Totalization Calibration</t>
+  </si>
+  <si>
+    <t>TG10/4 Ritter Totalization Calibration</t>
+  </si>
+  <si>
+    <t>Fluke</t>
+  </si>
+  <si>
+    <t>Ritter</t>
+  </si>
+  <si>
+    <t>Flow Rate (L/hr)</t>
+  </si>
+  <si>
+    <t>TG10/4 Ritter Flow Rate Calibration</t>
+  </si>
+  <si>
+    <t>Rate Calibration (Ideal HPLI Setting)</t>
+  </si>
+  <si>
+    <t>Rate Calibration (Upper HPLI Setting)</t>
+  </si>
+  <si>
+    <t>Rate Calibration (Lower HPLI Setting)</t>
+  </si>
+  <si>
+    <t>Timer (Minutes)</t>
+  </si>
+  <si>
+    <t>Totalization (L)</t>
+  </si>
+  <si>
+    <t>Totalization</t>
+  </si>
+  <si>
+    <t>Totalization Calbration (Ideal HPLI Setting)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t>Tol -</t>
+  </si>
+  <si>
+    <t>Tol +</t>
+  </si>
+  <si>
+    <t>As Found</t>
+  </si>
+  <si>
+    <t>As Left</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Verdict</t>
+  </si>
+  <si>
+    <t>Flow Rate</t>
+  </si>
+  <si>
+    <t>L/h</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Totalized flow for 15 mins</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Totalized flow for 100 mins at 1100 L/h</t>
+  </si>
+  <si>
+    <t>ltr/h</t>
+  </si>
+  <si>
+    <t>Lower limit Verification rate</t>
+  </si>
+  <si>
+    <t>Totalized flow</t>
+  </si>
+  <si>
+    <t>Upper Limit Verification rate</t>
+  </si>
+  <si>
+    <t>% Difference</t>
   </si>
 </sst>
 </file>
@@ -109,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -324,11 +456,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,6 +603,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,6 +635,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,6 +684,1720 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1.544.7HI'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1117.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1303.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1.544.7HI'!$I$2:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.61517429938482415</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26123301985370162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14144018333512864</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54755441034370911</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C90A-4AA3-85DE-72CA705DC347}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="603827632"/>
+        <c:axId val="603828112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="603827632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603828112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="603828112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603827632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'1.544.7HI'!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>325.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'1.544.7HI'!$I$6:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-0.54054054054054612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.3333333333324155E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.15000000000000568</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56750207061564417</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4320-49EE-B210-9D8C699E7066}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="603827632"/>
+        <c:axId val="603828112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="603827632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603828112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="603828112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603827632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,10 +2654,178 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF6517A-77C5-C2A6-BA67-9E36B5DC725D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9677401" y="476250"/>
+          <a:ext cx="2419350" cy="1209675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>CBRE Calibration Points</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>No STP</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Correction. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CF82300-6210-7E47-38F3-AE0AE19040C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89EF3CE9-F543-4AA5-85F9-3D2288322157}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -743,7 +2863,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -849,7 +2969,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -991,7 +3111,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1001,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE6164-C963-4648-B3F5-AC3D94478CBB}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,17 +3137,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-      <c r="N1" s="34" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="N1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="35"/>
+      <c r="O1" s="40"/>
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
       <c r="R1" s="24"/>
@@ -1180,21 +3300,21 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
       <c r="K10">
         <f>38.85*1040</f>
         <v>40404</v>
       </c>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="33"/>
+      <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1349,4 +3469,1293 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91721AE4-7256-461F-AAF4-A15885F728F8}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>15</v>
+      </c>
+      <c r="C3" s="13">
+        <f>(B3/60)*A3</f>
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="C4" s="13">
+        <f>(B4/60)*A4</f>
+        <v>6.25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>460</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15</v>
+      </c>
+      <c r="C12" s="13">
+        <f>(B12/60)*A12</f>
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2">
+        <v>15</v>
+      </c>
+      <c r="C13" s="13">
+        <f>(B13/60)*A13</f>
+        <v>6.25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="25"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B14" s="2">
+        <v>15</v>
+      </c>
+      <c r="C14" s="13">
+        <f>(B14/60)*A14</f>
+        <v>325</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>460</v>
+      </c>
+      <c r="B15" s="2">
+        <v>15</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="25"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>6</v>
+      </c>
+      <c r="B21" s="13">
+        <f>A21*0.0353147</f>
+        <v>0.21188819999999997</v>
+      </c>
+      <c r="C21" s="2">
+        <v>15</v>
+      </c>
+      <c r="D21" s="13">
+        <f>(C21/60)*B21</f>
+        <v>5.2972049999999993E-2</v>
+      </c>
+      <c r="E21" s="13">
+        <f>(C21/60)*A21</f>
+        <v>1.5</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <f t="shared" ref="B22:B24" si="0">A22*0.0353147</f>
+        <v>0.88286749999999992</v>
+      </c>
+      <c r="C22" s="2">
+        <v>15</v>
+      </c>
+      <c r="D22" s="13">
+        <f>(C22/60)*B22</f>
+        <v>0.22071687499999998</v>
+      </c>
+      <c r="E22" s="13">
+        <f>(C22/60)*A22</f>
+        <v>6.25</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>460</v>
+      </c>
+      <c r="B23" s="13">
+        <f t="shared" si="0"/>
+        <v>16.244761999999998</v>
+      </c>
+      <c r="C23" s="2">
+        <v>15</v>
+      </c>
+      <c r="D23" s="13">
+        <f>(C23/60)*B23</f>
+        <v>4.0611904999999995</v>
+      </c>
+      <c r="E23" s="13">
+        <f>(C23/60)*A23</f>
+        <v>115</v>
+      </c>
+      <c r="F23" s="2">
+        <v>30</v>
+      </c>
+      <c r="G23" s="2">
+        <v>850</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B24" s="13">
+        <f t="shared" si="0"/>
+        <v>38.846170000000001</v>
+      </c>
+      <c r="C24" s="2">
+        <v>15</v>
+      </c>
+      <c r="D24" s="13">
+        <f>(C24/60)*B24</f>
+        <v>9.7115425000000002</v>
+      </c>
+      <c r="E24" s="13">
+        <f>(C24/60)*A24</f>
+        <v>275</v>
+      </c>
+      <c r="F24" s="2">
+        <v>65</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1840</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>6</v>
+      </c>
+      <c r="B30" s="13">
+        <f>A30*0.0353147</f>
+        <v>0.21188819999999997</v>
+      </c>
+      <c r="C30" s="2">
+        <v>15</v>
+      </c>
+      <c r="D30" s="13">
+        <f>(C30/60)*B30</f>
+        <v>5.2972049999999993E-2</v>
+      </c>
+      <c r="E30" s="13">
+        <f>(C30/60)*A30</f>
+        <v>1.5</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>25</v>
+      </c>
+      <c r="B31" s="13">
+        <f t="shared" ref="B31:B34" si="1">A31*0.0353147</f>
+        <v>0.88286749999999992</v>
+      </c>
+      <c r="C31" s="2">
+        <v>15</v>
+      </c>
+      <c r="D31" s="13">
+        <f>(C31/60)*B31</f>
+        <v>0.22071687499999998</v>
+      </c>
+      <c r="E31" s="13">
+        <f>(C31/60)*A31</f>
+        <v>6.25</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>460</v>
+      </c>
+      <c r="B32" s="13">
+        <f t="shared" si="1"/>
+        <v>16.244761999999998</v>
+      </c>
+      <c r="C32" s="2">
+        <v>15</v>
+      </c>
+      <c r="D32" s="13">
+        <f>(C32/60)*B32</f>
+        <v>4.0611904999999995</v>
+      </c>
+      <c r="E32" s="13">
+        <f>(C32/60)*A32</f>
+        <v>115</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2">
+        <v>850</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B33" s="13">
+        <f t="shared" si="1"/>
+        <v>38.846170000000001</v>
+      </c>
+      <c r="C33" s="2">
+        <v>15</v>
+      </c>
+      <c r="D33" s="13">
+        <f>(C33/60)*B33</f>
+        <v>9.7115425000000002</v>
+      </c>
+      <c r="E33" s="13">
+        <f>(C33/60)*A33</f>
+        <v>275</v>
+      </c>
+      <c r="F33" s="2">
+        <v>30</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1840</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B34" s="13">
+        <f t="shared" si="1"/>
+        <v>45.909109999999998</v>
+      </c>
+      <c r="C34" s="2">
+        <v>15</v>
+      </c>
+      <c r="D34" s="13">
+        <f>(C34/60)*B34</f>
+        <v>11.4772775</v>
+      </c>
+      <c r="E34" s="13">
+        <f>(C34/60)*A34</f>
+        <v>325</v>
+      </c>
+      <c r="F34" s="2">
+        <v>65</v>
+      </c>
+      <c r="G34" s="31"/>
+      <c r="H34" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB26B767-F2DC-4386-AE9F-7408381851A9}">
+  <dimension ref="A1:L23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="6" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="48"/>
+      <c r="F2" s="42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>14</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>460</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="46"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="43"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="46"/>
+      <c r="J14">
+        <v>-0.1</v>
+      </c>
+      <c r="L14">
+        <f>J14-0.4</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="48"/>
+      <c r="F15" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>0.3</v>
+      </c>
+      <c r="L15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="L16">
+        <f>L15-L14</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32">
+        <v>15</v>
+      </c>
+      <c r="J17">
+        <f>J15-J14</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="43"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1100</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A9:F9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78B91E9-6932-45F6-A45B-818A36B79D58}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="50">
+        <v>14.63</v>
+      </c>
+      <c r="C2" s="50">
+        <v>14.48</v>
+      </c>
+      <c r="D2" s="50">
+        <v>14.78</v>
+      </c>
+      <c r="E2" s="50">
+        <v>14.72</v>
+      </c>
+      <c r="F2" s="50">
+        <v>14.72</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2">
+        <f>((F2/B2)-1)*100</f>
+        <v>0.61517429938482415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="50">
+        <v>478.5</v>
+      </c>
+      <c r="C3" s="50">
+        <v>473.72</v>
+      </c>
+      <c r="D3" s="50">
+        <v>483.29</v>
+      </c>
+      <c r="E3" s="50">
+        <v>479.75</v>
+      </c>
+      <c r="F3" s="50">
+        <v>479.75</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="50">
+        <f t="shared" ref="I3:I10" si="0">((F3/B3)-1)*100</f>
+        <v>0.26123301985370162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="50">
+        <v>1117.08</v>
+      </c>
+      <c r="C4" s="50">
+        <v>1105.9000000000001</v>
+      </c>
+      <c r="D4" s="50">
+        <v>1128.25</v>
+      </c>
+      <c r="E4" s="50">
+        <v>1118.6600000000001</v>
+      </c>
+      <c r="F4" s="50">
+        <v>1118.6600000000001</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="50">
+        <f t="shared" si="0"/>
+        <v>0.14144018333512864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="50">
+        <v>1303.98</v>
+      </c>
+      <c r="C5" s="50">
+        <v>1290.94</v>
+      </c>
+      <c r="D5" s="50">
+        <v>1317.02</v>
+      </c>
+      <c r="E5" s="50">
+        <v>1311.12</v>
+      </c>
+      <c r="F5" s="50">
+        <v>1311.12</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="50">
+        <f t="shared" si="0"/>
+        <v>0.54755441034370911</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="50">
+        <v>3.7</v>
+      </c>
+      <c r="C6" s="50">
+        <v>3.66</v>
+      </c>
+      <c r="D6" s="50">
+        <v>3.74</v>
+      </c>
+      <c r="E6" s="50">
+        <v>3.68</v>
+      </c>
+      <c r="F6" s="50">
+        <v>3.68</v>
+      </c>
+      <c r="G6" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="50">
+        <f t="shared" si="0"/>
+        <v>-0.54054054054054612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="50">
+        <v>120</v>
+      </c>
+      <c r="C7" s="50">
+        <v>118.8</v>
+      </c>
+      <c r="D7" s="50">
+        <v>121.2</v>
+      </c>
+      <c r="E7" s="50">
+        <v>119.9</v>
+      </c>
+      <c r="F7" s="50">
+        <v>119.9</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="50">
+        <f t="shared" si="0"/>
+        <v>-8.3333333333324155E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="50">
+        <v>280</v>
+      </c>
+      <c r="C8" s="50">
+        <v>277.2</v>
+      </c>
+      <c r="D8" s="50">
+        <v>282.8</v>
+      </c>
+      <c r="E8" s="50">
+        <v>279.58</v>
+      </c>
+      <c r="F8" s="50">
+        <v>279.58</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="50">
+        <f t="shared" si="0"/>
+        <v>-0.15000000000000568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="50">
+        <v>325.99</v>
+      </c>
+      <c r="C9" s="50">
+        <v>322.73</v>
+      </c>
+      <c r="D9" s="50">
+        <v>329.25</v>
+      </c>
+      <c r="E9" s="50">
+        <v>327.84</v>
+      </c>
+      <c r="F9" s="50">
+        <v>327.84</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="50">
+        <f t="shared" si="0"/>
+        <v>0.56750207061564417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="50">
+        <v>1916.99</v>
+      </c>
+      <c r="C10" s="50">
+        <v>1897.82</v>
+      </c>
+      <c r="D10" s="50">
+        <v>1936.16</v>
+      </c>
+      <c r="E10" s="50">
+        <v>1908.49</v>
+      </c>
+      <c r="F10" s="50">
+        <v>1908.49</v>
+      </c>
+      <c r="G10" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="50">
+        <f>((F10/B10)-1)*100</f>
+        <v>-0.4434034606335957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="50">
+        <v>1296.5999999999999</v>
+      </c>
+      <c r="C13" s="50">
+        <v>1283.6300000000001</v>
+      </c>
+      <c r="D13" s="50">
+        <v>1309.56</v>
+      </c>
+      <c r="E13" s="50">
+        <v>1286.49</v>
+      </c>
+      <c r="F13" s="50">
+        <v>1286.49</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="50">
+        <f t="shared" ref="I13:I16" si="1">((F13/B13)-1)*100</f>
+        <v>-0.77973160573807654</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="50">
+        <v>324.14999999999998</v>
+      </c>
+      <c r="C14" s="50">
+        <v>320.91000000000003</v>
+      </c>
+      <c r="D14" s="50">
+        <v>327.39</v>
+      </c>
+      <c r="E14" s="50">
+        <v>321.5</v>
+      </c>
+      <c r="F14" s="50">
+        <v>321.5</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="50">
+        <f t="shared" si="1"/>
+        <v>-0.81752275181242728</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="50">
+        <v>1311.78</v>
+      </c>
+      <c r="C15" s="50">
+        <v>1298.6600000000001</v>
+      </c>
+      <c r="D15" s="50">
+        <v>1324.9</v>
+      </c>
+      <c r="E15" s="50">
+        <v>1323.39</v>
+      </c>
+      <c r="F15" s="50">
+        <v>1323.39</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="50">
+        <f t="shared" si="1"/>
+        <v>0.8850569455244095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="50">
+        <v>327.95</v>
+      </c>
+      <c r="C16" s="50">
+        <v>324.67</v>
+      </c>
+      <c r="D16" s="50">
+        <v>331.22</v>
+      </c>
+      <c r="E16" s="50">
+        <v>330.82</v>
+      </c>
+      <c r="F16" s="50">
+        <v>330.82</v>
+      </c>
+      <c r="G16" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="50">
+        <f t="shared" si="1"/>
+        <v>0.87513340448239774</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>